<commit_message>
Urls anuncios, y otros errores arreglados
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -895,6 +895,28 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>23</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>aritz</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>28/05/2024</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>